<commit_message>
Final Upload Pandas HW due 10/12/2019
</commit_message>
<xml_diff>
--- a/Pandas HW/Part-1/Pandas_Mini_Project_Task_B/Resources/more_data_finished.xlsx
+++ b/Pandas HW/Part-1/Pandas_Mini_Project_Task_B/Resources/more_data_finished.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="28">
   <si>
     <t>Attended the Bootcamp</t>
   </si>
@@ -25,85 +25,79 @@
     <t>Result</t>
   </si>
   <si>
-    <t>1.67%</t>
-  </si>
-  <si>
-    <t>2.00%</t>
+    <t>0.60%</t>
+  </si>
+  <si>
+    <t>0.50%</t>
   </si>
   <si>
     <t>1.00%</t>
   </si>
   <si>
-    <t>1.12%</t>
-  </si>
-  <si>
-    <t>1.40%</t>
-  </si>
-  <si>
-    <t>1.10%</t>
-  </si>
-  <si>
-    <t>1.91%</t>
-  </si>
-  <si>
-    <t>1.50%</t>
-  </si>
-  <si>
-    <t>1.25%</t>
-  </si>
-  <si>
-    <t>1.83%</t>
-  </si>
-  <si>
-    <t>4.00%</t>
-  </si>
-  <si>
-    <t>1.64%</t>
-  </si>
-  <si>
-    <t>3.00%</t>
-  </si>
-  <si>
-    <t>1.17%</t>
-  </si>
-  <si>
-    <t>1.27%</t>
-  </si>
-  <si>
-    <t>1.08%</t>
-  </si>
-  <si>
-    <t>1.07%</t>
-  </si>
-  <si>
-    <t>1.82%</t>
-  </si>
-  <si>
-    <t>1.29%</t>
-  </si>
-  <si>
-    <t>1.16%</t>
-  </si>
-  <si>
-    <t>1.33%</t>
-  </si>
-  <si>
-    <t>1.11%</t>
-  </si>
-  <si>
-    <t>1.43%</t>
-  </si>
-  <si>
-    <t>1.20%</t>
-  </si>
-  <si>
-    <t>1.75%</t>
-  </si>
-  <si>
-    <t>1.23%</t>
-  </si>
-  <si>
-    <t>1.04%</t>
+    <t>0.89%</t>
+  </si>
+  <si>
+    <t>0.71%</t>
+  </si>
+  <si>
+    <t>0.91%</t>
+  </si>
+  <si>
+    <t>0.52%</t>
+  </si>
+  <si>
+    <t>0.67%</t>
+  </si>
+  <si>
+    <t>0.80%</t>
+  </si>
+  <si>
+    <t>0.55%</t>
+  </si>
+  <si>
+    <t>0.25%</t>
+  </si>
+  <si>
+    <t>0.61%</t>
+  </si>
+  <si>
+    <t>0.33%</t>
+  </si>
+  <si>
+    <t>0.85%</t>
+  </si>
+  <si>
+    <t>0.79%</t>
+  </si>
+  <si>
+    <t>0.93%</t>
+  </si>
+  <si>
+    <t>0.78%</t>
+  </si>
+  <si>
+    <t>0.86%</t>
+  </si>
+  <si>
+    <t>0.75%</t>
+  </si>
+  <si>
+    <t>0.90%</t>
+  </si>
+  <si>
+    <t>0.70%</t>
+  </si>
+  <si>
+    <t>0.83%</t>
+  </si>
+  <si>
+    <t>0.57%</t>
+  </si>
+  <si>
+    <t>0.81%</t>
+  </si>
+  <si>
+    <t>0.96%</t>
   </si>
 </sst>
 </file>
@@ -1102,7 +1096,7 @@
         <v>14</v>
       </c>
       <c r="C58" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1124,7 +1118,7 @@
         <v>11</v>
       </c>
       <c r="C60" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1135,7 +1129,7 @@
         <v>70</v>
       </c>
       <c r="C61" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1168,7 +1162,7 @@
         <v>27</v>
       </c>
       <c r="C64" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1179,7 +1173,7 @@
         <v>19</v>
       </c>
       <c r="C65" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1212,7 +1206,7 @@
         <v>3</v>
       </c>
       <c r="C68" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1300,7 +1294,7 @@
         <v>3</v>
       </c>
       <c r="C76" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1311,7 +1305,7 @@
         <v>18</v>
       </c>
       <c r="C77" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -1377,7 +1371,7 @@
         <v>14</v>
       </c>
       <c r="C83" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1443,7 +1437,7 @@
         <v>25</v>
       </c>
       <c r="C89" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -1476,7 +1470,7 @@
         <v>3</v>
       </c>
       <c r="C92" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -1487,7 +1481,7 @@
         <v>3</v>
       </c>
       <c r="C93" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -1520,7 +1514,7 @@
         <v>3</v>
       </c>
       <c r="C96" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -1564,7 +1558,7 @@
         <v>4</v>
       </c>
       <c r="C100" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -1619,7 +1613,7 @@
         <v>13</v>
       </c>
       <c r="C105" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -1630,7 +1624,7 @@
         <v>31</v>
       </c>
       <c r="C106" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -1641,7 +1635,7 @@
         <v>5</v>
       </c>
       <c r="C107" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -1652,7 +1646,7 @@
         <v>26</v>
       </c>
       <c r="C108" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="109" spans="1:3">

</xml_diff>